<commit_message>
Updated for importing Person records API
</commit_message>
<xml_diff>
--- a/src/test/resources/people_import.xlsx
+++ b/src/test/resources/people_import.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris.welch/workspace/personal/scoutsevents/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF7F31D-6C82-AE46-A371-18C4D0178B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F9BB58-729E-3347-BBD8-9F7760CAD91A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OSM Download" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'OSM Download'!$A$1:$Z$221</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,6 +30,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="107">
   <si>
     <t>First Name</t>
   </si>
@@ -356,6 +357,12 @@
   </si>
   <si>
     <t>Test9</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -749,7 +756,7 @@
   <dimension ref="A1:Z1066"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -839,7 +846,9 @@
       <c r="E3" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="F3" s="3"/>
+      <c r="F3" s="3" t="s">
+        <v>105</v>
+      </c>
       <c r="G3" s="3" t="s">
         <v>99</v>
       </c>
@@ -884,7 +893,7 @@
         <v>95</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>12</v>
+        <v>106</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>102</v>

</xml_diff>

<commit_message>
Adding Sub Camp field to Person
</commit_message>
<xml_diff>
--- a/src/test/resources/people_import.xlsx
+++ b/src/test/resources/people_import.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris.welch/workspace/personal/scoutsevents/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a3070294/workspace/personal/scouts/pentland_scouts_events_service/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F9BB58-729E-3347-BBD8-9F7760CAD91A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7E5B61-79E0-784E-8BC8-6AC393057A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="42400" yWindow="2880" windowWidth="28800" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OSM Download" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Changes" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'OSM Download'!$A$1:$Z$221</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'OSM Download'!$A$1:$AA$221</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="109">
   <si>
     <t>First Name</t>
   </si>
@@ -363,6 +363,12 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>SubCamp</t>
+  </si>
+  <si>
+    <t>Blue</t>
   </si>
 </sst>
 </file>
@@ -753,26 +759,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1066"/>
+  <dimension ref="A1:AA1066"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="16.6640625" customWidth="1"/>
     <col min="3" max="3" width="55.1640625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="40" customWidth="1"/>
-    <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="44.6640625" customWidth="1"/>
-    <col min="8" max="8" width="125" customWidth="1"/>
-    <col min="9" max="9" width="81.33203125" customWidth="1"/>
-    <col min="10" max="26" width="8.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="6" width="40" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
+    <col min="8" max="8" width="44.6640625" customWidth="1"/>
+    <col min="9" max="9" width="125" customWidth="1"/>
+    <col min="10" max="10" width="81.33203125" customWidth="1"/>
+    <col min="11" max="27" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -783,25 +790,28 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>90</v>
       </c>
@@ -812,25 +822,28 @@
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="F2" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -841,24 +854,26 @@
         <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="F3" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="J3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
@@ -875,8 +890,9 @@
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
       <c r="Z3" s="4"/>
-    </row>
-    <row r="4" spans="1:26" ht="11" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA3" s="4"/>
+    </row>
+    <row r="4" spans="1:27" ht="11" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>93</v>
       </c>
@@ -887,25 +903,28 @@
         <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="F4" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -915,8 +934,9 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -926,8 +946,9 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -937,8 +958,9 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -948,8 +970,9 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -959,7 +982,7 @@
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
-      <c r="J9" s="2"/>
+      <c r="J9" s="5"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -976,8 +999,9 @@
       <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA9" s="2"/>
+    </row>
+    <row r="10" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -987,8 +1011,9 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -998,8 +1023,9 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1009,8 +1035,9 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1020,8 +1047,9 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1031,8 +1059,9 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1042,8 +1071,9 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1053,8 +1083,9 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1064,8 +1095,9 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J17" s="2"/>
+    </row>
+    <row r="18" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1075,8 +1107,9 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
-    </row>
-    <row r="19" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1086,8 +1119,9 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
-    </row>
-    <row r="20" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J19" s="2"/>
+    </row>
+    <row r="20" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1097,7 +1131,7 @@
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
-      <c r="J20" s="4"/>
+      <c r="J20" s="3"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
@@ -1114,8 +1148,9 @@
       <c r="X20" s="4"/>
       <c r="Y20" s="4"/>
       <c r="Z20" s="4"/>
-    </row>
-    <row r="21" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA20" s="4"/>
+    </row>
+    <row r="21" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1142,8 +1177,9 @@
       <c r="X21" s="2"/>
       <c r="Y21" s="2"/>
       <c r="Z21" s="2"/>
-    </row>
-    <row r="22" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA21" s="2"/>
+    </row>
+    <row r="22" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1153,8 +1189,9 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
-    </row>
-    <row r="23" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1164,8 +1201,9 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
-    </row>
-    <row r="24" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J23" s="2"/>
+    </row>
+    <row r="24" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -1175,8 +1213,9 @@
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
-    </row>
-    <row r="25" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J24" s="5"/>
+    </row>
+    <row r="25" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1186,8 +1225,9 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
-    </row>
-    <row r="26" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J25" s="2"/>
+    </row>
+    <row r="26" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1197,8 +1237,9 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
-    </row>
-    <row r="27" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J26" s="2"/>
+    </row>
+    <row r="27" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1208,8 +1249,9 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
-    </row>
-    <row r="28" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J27" s="2"/>
+    </row>
+    <row r="28" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1219,8 +1261,9 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
-    </row>
-    <row r="29" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J28" s="2"/>
+    </row>
+    <row r="29" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1247,8 +1290,9 @@
       <c r="X29" s="2"/>
       <c r="Y29" s="2"/>
       <c r="Z29" s="2"/>
-    </row>
-    <row r="30" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA29" s="2"/>
+    </row>
+    <row r="30" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1258,8 +1302,9 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
-    </row>
-    <row r="31" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J30" s="2"/>
+    </row>
+    <row r="31" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1269,8 +1314,9 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
-    </row>
-    <row r="32" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J31" s="2"/>
+    </row>
+    <row r="32" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -1280,8 +1326,9 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
-    </row>
-    <row r="33" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J32" s="2"/>
+    </row>
+    <row r="33" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -1291,8 +1338,9 @@
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
-    </row>
-    <row r="34" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J33" s="5"/>
+    </row>
+    <row r="34" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -1302,8 +1350,9 @@
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
-    </row>
-    <row r="35" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J34" s="5"/>
+    </row>
+    <row r="35" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1313,8 +1362,9 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
-    </row>
-    <row r="36" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J35" s="2"/>
+    </row>
+    <row r="36" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1341,8 +1391,9 @@
       <c r="X36" s="2"/>
       <c r="Y36" s="2"/>
       <c r="Z36" s="2"/>
-    </row>
-    <row r="37" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA36" s="2"/>
+    </row>
+    <row r="37" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1352,8 +1403,9 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
-    </row>
-    <row r="38" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J37" s="2"/>
+    </row>
+    <row r="38" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1363,8 +1415,9 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
-    </row>
-    <row r="39" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J38" s="2"/>
+    </row>
+    <row r="39" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1374,8 +1427,9 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
-    </row>
-    <row r="40" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J39" s="2"/>
+    </row>
+    <row r="40" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1385,8 +1439,9 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
-    </row>
-    <row r="41" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J40" s="2"/>
+    </row>
+    <row r="41" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1396,8 +1451,9 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
-    </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J41" s="2"/>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -1407,8 +1463,9 @@
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
-    </row>
-    <row r="43" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J42" s="5"/>
+    </row>
+    <row r="43" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1418,8 +1475,9 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
-    </row>
-    <row r="44" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J43" s="2"/>
+    </row>
+    <row r="44" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -1429,8 +1487,9 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
-    </row>
-    <row r="45" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J44" s="2"/>
+    </row>
+    <row r="45" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -1440,8 +1499,9 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
-    </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J45" s="2"/>
+    </row>
+    <row r="46" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
@@ -1451,8 +1511,9 @@
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
-    </row>
-    <row r="47" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J46" s="5"/>
+    </row>
+    <row r="47" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -1462,8 +1523,9 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
-    </row>
-    <row r="48" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J47" s="2"/>
+    </row>
+    <row r="48" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -1473,8 +1535,9 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
-    </row>
-    <row r="49" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J48" s="2"/>
+    </row>
+    <row r="49" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -1484,8 +1547,9 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
-    </row>
-    <row r="50" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J49" s="2"/>
+    </row>
+    <row r="50" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -1495,8 +1559,9 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
-    </row>
-    <row r="51" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J50" s="2"/>
+    </row>
+    <row r="51" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -1506,8 +1571,9 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
-    </row>
-    <row r="52" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J51" s="2"/>
+    </row>
+    <row r="52" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -1517,8 +1583,9 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
-    </row>
-    <row r="53" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J52" s="2"/>
+    </row>
+    <row r="53" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -1528,8 +1595,9 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
-    </row>
-    <row r="54" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J53" s="2"/>
+    </row>
+    <row r="54" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -1539,8 +1607,9 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
-    </row>
-    <row r="55" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J54" s="2"/>
+    </row>
+    <row r="55" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -1550,8 +1619,9 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
-    </row>
-    <row r="56" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J55" s="2"/>
+    </row>
+    <row r="56" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -1578,8 +1648,9 @@
       <c r="X56" s="2"/>
       <c r="Y56" s="2"/>
       <c r="Z56" s="2"/>
-    </row>
-    <row r="57" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA56" s="2"/>
+    </row>
+    <row r="57" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -1606,8 +1677,9 @@
       <c r="X57" s="4"/>
       <c r="Y57" s="4"/>
       <c r="Z57" s="4"/>
-    </row>
-    <row r="58" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA57" s="4"/>
+    </row>
+    <row r="58" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -1617,8 +1689,9 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
-    </row>
-    <row r="59" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J58" s="2"/>
+    </row>
+    <row r="59" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="5"/>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
@@ -1628,7 +1701,7 @@
       <c r="G59" s="5"/>
       <c r="H59" s="5"/>
       <c r="I59" s="5"/>
-      <c r="J59" s="2"/>
+      <c r="J59" s="5"/>
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
       <c r="M59" s="2"/>
@@ -1645,8 +1718,9 @@
       <c r="X59" s="2"/>
       <c r="Y59" s="2"/>
       <c r="Z59" s="2"/>
-    </row>
-    <row r="60" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA59" s="2"/>
+    </row>
+    <row r="60" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -1656,8 +1730,9 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
-    </row>
-    <row r="61" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J60" s="2"/>
+    </row>
+    <row r="61" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -1684,8 +1759,9 @@
       <c r="X61" s="2"/>
       <c r="Y61" s="2"/>
       <c r="Z61" s="2"/>
-    </row>
-    <row r="62" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA61" s="2"/>
+    </row>
+    <row r="62" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -1695,8 +1771,9 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
-    </row>
-    <row r="63" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J62" s="2"/>
+    </row>
+    <row r="63" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="5"/>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
@@ -1706,8 +1783,9 @@
       <c r="G63" s="5"/>
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
-    </row>
-    <row r="64" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J63" s="5"/>
+    </row>
+    <row r="64" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -1717,8 +1795,9 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
-    </row>
-    <row r="65" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J64" s="2"/>
+    </row>
+    <row r="65" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="5"/>
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
@@ -1728,7 +1807,7 @@
       <c r="G65" s="5"/>
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>
-      <c r="J65" s="2"/>
+      <c r="J65" s="5"/>
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
       <c r="M65" s="2"/>
@@ -1745,8 +1824,9 @@
       <c r="X65" s="2"/>
       <c r="Y65" s="2"/>
       <c r="Z65" s="2"/>
-    </row>
-    <row r="66" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA65" s="2"/>
+    </row>
+    <row r="66" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="5"/>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
@@ -1756,8 +1836,9 @@
       <c r="G66" s="5"/>
       <c r="H66" s="5"/>
       <c r="I66" s="5"/>
-    </row>
-    <row r="67" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J66" s="5"/>
+    </row>
+    <row r="67" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="5"/>
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
@@ -1767,8 +1848,9 @@
       <c r="G67" s="5"/>
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
-    </row>
-    <row r="68" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J67" s="5"/>
+    </row>
+    <row r="68" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -1776,9 +1858,10 @@
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
-      <c r="I68" s="2"/>
-    </row>
-    <row r="69" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H68" s="2"/>
+      <c r="J68" s="2"/>
+    </row>
+    <row r="69" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="5"/>
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
@@ -1788,8 +1871,9 @@
       <c r="G69" s="5"/>
       <c r="H69" s="5"/>
       <c r="I69" s="5"/>
-    </row>
-    <row r="70" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J69" s="5"/>
+    </row>
+    <row r="70" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -1799,8 +1883,9 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
       <c r="I70" s="2"/>
-    </row>
-    <row r="71" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J70" s="2"/>
+    </row>
+    <row r="71" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -1810,8 +1895,9 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
       <c r="I71" s="2"/>
-    </row>
-    <row r="72" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J71" s="2"/>
+    </row>
+    <row r="72" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="5"/>
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
@@ -1821,8 +1907,9 @@
       <c r="G72" s="5"/>
       <c r="H72" s="5"/>
       <c r="I72" s="5"/>
-    </row>
-    <row r="73" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J72" s="5"/>
+    </row>
+    <row r="73" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -1832,8 +1919,9 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
       <c r="I73" s="2"/>
-    </row>
-    <row r="74" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J73" s="2"/>
+    </row>
+    <row r="74" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -1843,8 +1931,9 @@
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
       <c r="I74" s="2"/>
-    </row>
-    <row r="75" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J74" s="2"/>
+    </row>
+    <row r="75" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -1854,8 +1943,9 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
       <c r="I75" s="2"/>
-    </row>
-    <row r="76" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J75" s="2"/>
+    </row>
+    <row r="76" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -1865,8 +1955,9 @@
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
       <c r="I76" s="2"/>
-    </row>
-    <row r="77" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J76" s="2"/>
+    </row>
+    <row r="77" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="5"/>
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
@@ -1876,8 +1967,9 @@
       <c r="G77" s="5"/>
       <c r="H77" s="5"/>
       <c r="I77" s="5"/>
-    </row>
-    <row r="78" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J77" s="5"/>
+    </row>
+    <row r="78" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -1887,8 +1979,9 @@
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
       <c r="I78" s="2"/>
-    </row>
-    <row r="79" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J78" s="2"/>
+    </row>
+    <row r="79" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="5"/>
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
@@ -1898,8 +1991,9 @@
       <c r="G79" s="5"/>
       <c r="H79" s="5"/>
       <c r="I79" s="5"/>
-    </row>
-    <row r="80" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J79" s="5"/>
+    </row>
+    <row r="80" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="5"/>
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
@@ -1909,8 +2003,9 @@
       <c r="G80" s="5"/>
       <c r="H80" s="5"/>
       <c r="I80" s="5"/>
-    </row>
-    <row r="81" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J80" s="5"/>
+    </row>
+    <row r="81" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -1920,8 +2015,9 @@
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
       <c r="I81" s="2"/>
-    </row>
-    <row r="82" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J81" s="2"/>
+    </row>
+    <row r="82" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -1931,8 +2027,9 @@
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
       <c r="I82" s="2"/>
-    </row>
-    <row r="83" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J82" s="2"/>
+    </row>
+    <row r="83" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="5"/>
       <c r="B83" s="5"/>
       <c r="C83" s="5"/>
@@ -1942,7 +2039,7 @@
       <c r="G83" s="5"/>
       <c r="H83" s="5"/>
       <c r="I83" s="5"/>
-      <c r="J83" s="2"/>
+      <c r="J83" s="5"/>
       <c r="K83" s="2"/>
       <c r="L83" s="2"/>
       <c r="M83" s="2"/>
@@ -1959,8 +2056,9 @@
       <c r="X83" s="2"/>
       <c r="Y83" s="2"/>
       <c r="Z83" s="2"/>
-    </row>
-    <row r="84" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA83" s="2"/>
+    </row>
+    <row r="84" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -1970,8 +2068,9 @@
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
       <c r="I84" s="2"/>
-    </row>
-    <row r="85" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J84" s="2"/>
+    </row>
+    <row r="85" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -1981,8 +2080,9 @@
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
       <c r="I85" s="2"/>
-    </row>
-    <row r="86" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J85" s="2"/>
+    </row>
+    <row r="86" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -1992,8 +2092,9 @@
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
       <c r="I86" s="2"/>
-    </row>
-    <row r="87" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J86" s="2"/>
+    </row>
+    <row r="87" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -2003,8 +2104,9 @@
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
       <c r="I87" s="2"/>
-    </row>
-    <row r="88" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J87" s="2"/>
+    </row>
+    <row r="88" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -2014,8 +2116,9 @@
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
       <c r="I88" s="2"/>
-    </row>
-    <row r="89" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J88" s="2"/>
+    </row>
+    <row r="89" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="5"/>
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
@@ -2025,8 +2128,9 @@
       <c r="G89" s="5"/>
       <c r="H89" s="5"/>
       <c r="I89" s="5"/>
-    </row>
-    <row r="90" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J89" s="5"/>
+    </row>
+    <row r="90" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="5"/>
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
@@ -2036,8 +2140,9 @@
       <c r="G90" s="5"/>
       <c r="H90" s="5"/>
       <c r="I90" s="5"/>
-    </row>
-    <row r="91" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J90" s="5"/>
+    </row>
+    <row r="91" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="5"/>
       <c r="B91" s="5"/>
       <c r="C91" s="5"/>
@@ -2047,7 +2152,7 @@
       <c r="G91" s="5"/>
       <c r="H91" s="5"/>
       <c r="I91" s="5"/>
-      <c r="J91" s="2"/>
+      <c r="J91" s="5"/>
       <c r="K91" s="2"/>
       <c r="L91" s="2"/>
       <c r="M91" s="2"/>
@@ -2064,8 +2169,9 @@
       <c r="X91" s="2"/>
       <c r="Y91" s="2"/>
       <c r="Z91" s="2"/>
-    </row>
-    <row r="92" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA91" s="2"/>
+    </row>
+    <row r="92" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="3"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
@@ -2075,7 +2181,7 @@
       <c r="G92" s="3"/>
       <c r="H92" s="3"/>
       <c r="I92" s="3"/>
-      <c r="J92" s="4"/>
+      <c r="J92" s="3"/>
       <c r="K92" s="4"/>
       <c r="L92" s="4"/>
       <c r="M92" s="4"/>
@@ -2092,8 +2198,9 @@
       <c r="X92" s="4"/>
       <c r="Y92" s="4"/>
       <c r="Z92" s="4"/>
-    </row>
-    <row r="93" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA92" s="4"/>
+    </row>
+    <row r="93" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="5"/>
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
@@ -2103,7 +2210,7 @@
       <c r="G93" s="5"/>
       <c r="H93" s="5"/>
       <c r="I93" s="5"/>
-      <c r="J93" s="2"/>
+      <c r="J93" s="5"/>
       <c r="K93" s="2"/>
       <c r="L93" s="2"/>
       <c r="M93" s="2"/>
@@ -2120,8 +2227,9 @@
       <c r="X93" s="2"/>
       <c r="Y93" s="2"/>
       <c r="Z93" s="2"/>
-    </row>
-    <row r="94" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA93" s="2"/>
+    </row>
+    <row r="94" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="5"/>
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
@@ -2131,8 +2239,9 @@
       <c r="G94" s="5"/>
       <c r="H94" s="5"/>
       <c r="I94" s="5"/>
-    </row>
-    <row r="95" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J94" s="5"/>
+    </row>
+    <row r="95" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="3"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
@@ -2142,7 +2251,7 @@
       <c r="G95" s="3"/>
       <c r="H95" s="3"/>
       <c r="I95" s="3"/>
-      <c r="J95" s="4"/>
+      <c r="J95" s="3"/>
       <c r="K95" s="4"/>
       <c r="L95" s="4"/>
       <c r="M95" s="4"/>
@@ -2159,8 +2268,9 @@
       <c r="X95" s="4"/>
       <c r="Y95" s="4"/>
       <c r="Z95" s="4"/>
-    </row>
-    <row r="96" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA95" s="4"/>
+    </row>
+    <row r="96" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -2170,8 +2280,9 @@
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
       <c r="I96" s="2"/>
-    </row>
-    <row r="97" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J96" s="2"/>
+    </row>
+    <row r="97" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -2181,8 +2292,9 @@
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
       <c r="I97" s="2"/>
-    </row>
-    <row r="98" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J97" s="2"/>
+    </row>
+    <row r="98" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="5"/>
       <c r="B98" s="5"/>
       <c r="C98" s="5"/>
@@ -2192,8 +2304,9 @@
       <c r="G98" s="5"/>
       <c r="H98" s="5"/>
       <c r="I98" s="5"/>
-    </row>
-    <row r="99" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J98" s="5"/>
+    </row>
+    <row r="99" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -2203,8 +2316,9 @@
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
       <c r="I99" s="2"/>
-    </row>
-    <row r="100" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J99" s="2"/>
+    </row>
+    <row r="100" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -2214,8 +2328,9 @@
       <c r="G100" s="2"/>
       <c r="H100" s="2"/>
       <c r="I100" s="2"/>
-    </row>
-    <row r="101" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J100" s="2"/>
+    </row>
+    <row r="101" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -2225,8 +2340,9 @@
       <c r="G101" s="2"/>
       <c r="H101" s="2"/>
       <c r="I101" s="2"/>
-    </row>
-    <row r="102" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J101" s="2"/>
+    </row>
+    <row r="102" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="5"/>
       <c r="B102" s="5"/>
       <c r="C102" s="5"/>
@@ -2236,7 +2352,7 @@
       <c r="G102" s="5"/>
       <c r="H102" s="5"/>
       <c r="I102" s="5"/>
-      <c r="J102" s="4"/>
+      <c r="J102" s="5"/>
       <c r="K102" s="4"/>
       <c r="L102" s="4"/>
       <c r="M102" s="4"/>
@@ -2253,8 +2369,9 @@
       <c r="X102" s="4"/>
       <c r="Y102" s="4"/>
       <c r="Z102" s="4"/>
-    </row>
-    <row r="103" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA102" s="4"/>
+    </row>
+    <row r="103" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="4"/>
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
@@ -2281,8 +2398,9 @@
       <c r="X103" s="4"/>
       <c r="Y103" s="4"/>
       <c r="Z103" s="4"/>
-    </row>
-    <row r="104" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA103" s="4"/>
+    </row>
+    <row r="104" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -2292,8 +2410,9 @@
       <c r="G104" s="2"/>
       <c r="H104" s="2"/>
       <c r="I104" s="2"/>
-    </row>
-    <row r="105" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J104" s="2"/>
+    </row>
+    <row r="105" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -2303,8 +2422,9 @@
       <c r="G105" s="2"/>
       <c r="H105" s="2"/>
       <c r="I105" s="2"/>
-    </row>
-    <row r="106" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J105" s="2"/>
+    </row>
+    <row r="106" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -2314,8 +2434,9 @@
       <c r="G106" s="2"/>
       <c r="H106" s="2"/>
       <c r="I106" s="2"/>
-    </row>
-    <row r="107" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J106" s="2"/>
+    </row>
+    <row r="107" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -2325,8 +2446,9 @@
       <c r="G107" s="2"/>
       <c r="H107" s="2"/>
       <c r="I107" s="2"/>
-    </row>
-    <row r="108" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J107" s="2"/>
+    </row>
+    <row r="108" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -2336,8 +2458,9 @@
       <c r="G108" s="2"/>
       <c r="H108" s="2"/>
       <c r="I108" s="2"/>
-    </row>
-    <row r="109" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J108" s="2"/>
+    </row>
+    <row r="109" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="5"/>
       <c r="B109" s="5"/>
       <c r="C109" s="5"/>
@@ -2347,8 +2470,9 @@
       <c r="G109" s="5"/>
       <c r="H109" s="5"/>
       <c r="I109" s="5"/>
-    </row>
-    <row r="110" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J109" s="5"/>
+    </row>
+    <row r="110" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="5"/>
       <c r="B110" s="5"/>
       <c r="C110" s="5"/>
@@ -2358,8 +2482,9 @@
       <c r="G110" s="5"/>
       <c r="H110" s="5"/>
       <c r="I110" s="5"/>
-    </row>
-    <row r="111" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J110" s="5"/>
+    </row>
+    <row r="111" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -2367,9 +2492,10 @@
       <c r="E111" s="2"/>
       <c r="F111" s="2"/>
       <c r="G111" s="2"/>
-      <c r="I111" s="2"/>
-    </row>
-    <row r="112" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H111" s="2"/>
+      <c r="J111" s="2"/>
+    </row>
+    <row r="112" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -2379,8 +2505,9 @@
       <c r="G112" s="2"/>
       <c r="H112" s="2"/>
       <c r="I112" s="2"/>
-    </row>
-    <row r="113" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J112" s="2"/>
+    </row>
+    <row r="113" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="5"/>
       <c r="B113" s="5"/>
       <c r="C113" s="5"/>
@@ -2390,8 +2517,9 @@
       <c r="G113" s="5"/>
       <c r="H113" s="5"/>
       <c r="I113" s="5"/>
-    </row>
-    <row r="114" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J113" s="5"/>
+    </row>
+    <row r="114" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -2401,8 +2529,9 @@
       <c r="G114" s="2"/>
       <c r="H114" s="2"/>
       <c r="I114" s="2"/>
-    </row>
-    <row r="115" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J114" s="2"/>
+    </row>
+    <row r="115" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="4"/>
       <c r="B115" s="4"/>
       <c r="C115" s="4"/>
@@ -2429,8 +2558,9 @@
       <c r="X115" s="4"/>
       <c r="Y115" s="4"/>
       <c r="Z115" s="4"/>
-    </row>
-    <row r="116" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA115" s="4"/>
+    </row>
+    <row r="116" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -2438,9 +2568,10 @@
       <c r="E116" s="2"/>
       <c r="F116" s="2"/>
       <c r="G116" s="2"/>
-      <c r="I116" s="2"/>
-    </row>
-    <row r="117" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H116" s="2"/>
+      <c r="J116" s="2"/>
+    </row>
+    <row r="117" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -2450,8 +2581,9 @@
       <c r="G117" s="2"/>
       <c r="H117" s="2"/>
       <c r="I117" s="2"/>
-    </row>
-    <row r="118" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J117" s="2"/>
+    </row>
+    <row r="118" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -2461,8 +2593,9 @@
       <c r="G118" s="2"/>
       <c r="H118" s="2"/>
       <c r="I118" s="2"/>
-    </row>
-    <row r="119" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J118" s="2"/>
+    </row>
+    <row r="119" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -2472,8 +2605,9 @@
       <c r="G119" s="2"/>
       <c r="H119" s="2"/>
       <c r="I119" s="2"/>
-    </row>
-    <row r="120" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J119" s="2"/>
+    </row>
+    <row r="120" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -2483,8 +2617,9 @@
       <c r="G120" s="2"/>
       <c r="H120" s="2"/>
       <c r="I120" s="2"/>
-    </row>
-    <row r="121" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J120" s="2"/>
+    </row>
+    <row r="121" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
@@ -2494,8 +2629,9 @@
       <c r="G121" s="2"/>
       <c r="H121" s="2"/>
       <c r="I121" s="2"/>
-    </row>
-    <row r="122" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J121" s="2"/>
+    </row>
+    <row r="122" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -2505,8 +2641,9 @@
       <c r="G122" s="2"/>
       <c r="H122" s="2"/>
       <c r="I122" s="2"/>
-    </row>
-    <row r="123" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J122" s="2"/>
+    </row>
+    <row r="123" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -2516,8 +2653,9 @@
       <c r="G123" s="2"/>
       <c r="H123" s="2"/>
       <c r="I123" s="2"/>
-    </row>
-    <row r="124" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J123" s="2"/>
+    </row>
+    <row r="124" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -2527,8 +2665,9 @@
       <c r="G124" s="2"/>
       <c r="H124" s="2"/>
       <c r="I124" s="2"/>
-    </row>
-    <row r="125" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J124" s="2"/>
+    </row>
+    <row r="125" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -2538,8 +2677,9 @@
       <c r="G125" s="2"/>
       <c r="H125" s="2"/>
       <c r="I125" s="2"/>
-    </row>
-    <row r="126" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J125" s="2"/>
+    </row>
+    <row r="126" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="5"/>
       <c r="B126" s="5"/>
       <c r="C126" s="5"/>
@@ -2549,8 +2689,9 @@
       <c r="G126" s="5"/>
       <c r="H126" s="5"/>
       <c r="I126" s="5"/>
-    </row>
-    <row r="127" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J126" s="5"/>
+    </row>
+    <row r="127" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -2560,8 +2701,9 @@
       <c r="G127" s="2"/>
       <c r="H127" s="2"/>
       <c r="I127" s="2"/>
-    </row>
-    <row r="128" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J127" s="2"/>
+    </row>
+    <row r="128" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="5"/>
       <c r="B128" s="5"/>
       <c r="C128" s="5"/>
@@ -2571,8 +2713,9 @@
       <c r="G128" s="5"/>
       <c r="H128" s="5"/>
       <c r="I128" s="5"/>
-    </row>
-    <row r="129" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J128" s="5"/>
+    </row>
+    <row r="129" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="5"/>
       <c r="B129" s="5"/>
       <c r="C129" s="5"/>
@@ -2582,8 +2725,9 @@
       <c r="G129" s="5"/>
       <c r="H129" s="5"/>
       <c r="I129" s="5"/>
-    </row>
-    <row r="130" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J129" s="5"/>
+    </row>
+    <row r="130" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="5"/>
       <c r="B130" s="5"/>
       <c r="C130" s="5"/>
@@ -2593,8 +2737,9 @@
       <c r="G130" s="5"/>
       <c r="H130" s="5"/>
       <c r="I130" s="5"/>
-    </row>
-    <row r="131" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J130" s="5"/>
+    </row>
+    <row r="131" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="5"/>
       <c r="B131" s="5"/>
       <c r="C131" s="5"/>
@@ -2604,7 +2749,7 @@
       <c r="G131" s="5"/>
       <c r="H131" s="5"/>
       <c r="I131" s="5"/>
-      <c r="J131" s="2"/>
+      <c r="J131" s="5"/>
       <c r="K131" s="2"/>
       <c r="L131" s="2"/>
       <c r="M131" s="2"/>
@@ -2621,8 +2766,9 @@
       <c r="X131" s="2"/>
       <c r="Y131" s="2"/>
       <c r="Z131" s="2"/>
-    </row>
-    <row r="132" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA131" s="2"/>
+    </row>
+    <row r="132" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="5"/>
       <c r="B132" s="5"/>
       <c r="C132" s="5"/>
@@ -2632,8 +2778,9 @@
       <c r="G132" s="5"/>
       <c r="H132" s="5"/>
       <c r="I132" s="5"/>
-    </row>
-    <row r="133" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J132" s="5"/>
+    </row>
+    <row r="133" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="5"/>
       <c r="B133" s="5"/>
       <c r="C133" s="5"/>
@@ -2643,8 +2790,9 @@
       <c r="G133" s="5"/>
       <c r="H133" s="5"/>
       <c r="I133" s="5"/>
-    </row>
-    <row r="134" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J133" s="5"/>
+    </row>
+    <row r="134" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="5"/>
       <c r="B134" s="5"/>
       <c r="C134" s="5"/>
@@ -2654,7 +2802,7 @@
       <c r="G134" s="5"/>
       <c r="H134" s="5"/>
       <c r="I134" s="5"/>
-      <c r="J134" s="2"/>
+      <c r="J134" s="5"/>
       <c r="K134" s="2"/>
       <c r="L134" s="2"/>
       <c r="M134" s="2"/>
@@ -2671,8 +2819,9 @@
       <c r="X134" s="2"/>
       <c r="Y134" s="2"/>
       <c r="Z134" s="2"/>
-    </row>
-    <row r="135" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA134" s="2"/>
+    </row>
+    <row r="135" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="3"/>
       <c r="B135" s="3"/>
       <c r="C135" s="3"/>
@@ -2682,7 +2831,7 @@
       <c r="G135" s="3"/>
       <c r="H135" s="3"/>
       <c r="I135" s="3"/>
-      <c r="J135" s="4"/>
+      <c r="J135" s="3"/>
       <c r="K135" s="4"/>
       <c r="L135" s="4"/>
       <c r="M135" s="4"/>
@@ -2699,8 +2848,9 @@
       <c r="X135" s="4"/>
       <c r="Y135" s="4"/>
       <c r="Z135" s="4"/>
-    </row>
-    <row r="136" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA135" s="4"/>
+    </row>
+    <row r="136" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="5"/>
       <c r="B136" s="5"/>
       <c r="C136" s="5"/>
@@ -2710,8 +2860,9 @@
       <c r="G136" s="5"/>
       <c r="H136" s="5"/>
       <c r="I136" s="5"/>
-    </row>
-    <row r="137" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J136" s="5"/>
+    </row>
+    <row r="137" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="5"/>
       <c r="B137" s="5"/>
       <c r="C137" s="5"/>
@@ -2721,8 +2872,9 @@
       <c r="G137" s="5"/>
       <c r="H137" s="5"/>
       <c r="I137" s="5"/>
-    </row>
-    <row r="138" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J137" s="5"/>
+    </row>
+    <row r="138" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="5"/>
       <c r="B138" s="5"/>
       <c r="C138" s="5"/>
@@ -2732,8 +2884,9 @@
       <c r="G138" s="5"/>
       <c r="H138" s="5"/>
       <c r="I138" s="5"/>
-    </row>
-    <row r="139" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J138" s="5"/>
+    </row>
+    <row r="139" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="5"/>
       <c r="B139" s="5"/>
       <c r="C139" s="5"/>
@@ -2743,8 +2896,9 @@
       <c r="G139" s="5"/>
       <c r="H139" s="5"/>
       <c r="I139" s="5"/>
-    </row>
-    <row r="140" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J139" s="5"/>
+    </row>
+    <row r="140" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A140" s="5"/>
       <c r="B140" s="5"/>
       <c r="C140" s="5"/>
@@ -2754,8 +2908,9 @@
       <c r="G140" s="5"/>
       <c r="H140" s="5"/>
       <c r="I140" s="5"/>
-    </row>
-    <row r="141" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J140" s="5"/>
+    </row>
+    <row r="141" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="5"/>
       <c r="B141" s="5"/>
       <c r="C141" s="5"/>
@@ -2765,8 +2920,9 @@
       <c r="G141" s="5"/>
       <c r="H141" s="5"/>
       <c r="I141" s="5"/>
-    </row>
-    <row r="142" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J141" s="5"/>
+    </row>
+    <row r="142" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="5"/>
       <c r="B142" s="5"/>
       <c r="C142" s="5"/>
@@ -2776,8 +2932,9 @@
       <c r="G142" s="5"/>
       <c r="H142" s="5"/>
       <c r="I142" s="5"/>
-    </row>
-    <row r="143" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J142" s="5"/>
+    </row>
+    <row r="143" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="2"/>
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
@@ -2787,8 +2944,9 @@
       <c r="G143" s="2"/>
       <c r="H143" s="2"/>
       <c r="I143" s="2"/>
-    </row>
-    <row r="144" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J143" s="2"/>
+    </row>
+    <row r="144" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A144" s="5"/>
       <c r="B144" s="5"/>
       <c r="C144" s="5"/>
@@ -2798,8 +2956,9 @@
       <c r="G144" s="5"/>
       <c r="H144" s="5"/>
       <c r="I144" s="5"/>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J144" s="5"/>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A145" s="5"/>
       <c r="B145" s="5"/>
       <c r="C145" s="5"/>
@@ -2809,8 +2968,9 @@
       <c r="G145" s="5"/>
       <c r="H145" s="5"/>
       <c r="I145" s="5"/>
-    </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J145" s="5"/>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A146" s="5"/>
       <c r="B146" s="5"/>
       <c r="C146" s="5"/>
@@ -2820,8 +2980,9 @@
       <c r="G146" s="5"/>
       <c r="H146" s="5"/>
       <c r="I146" s="5"/>
-    </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J146" s="5"/>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A147" s="5"/>
       <c r="B147" s="5"/>
       <c r="C147" s="5"/>
@@ -2831,8 +2992,9 @@
       <c r="G147" s="5"/>
       <c r="H147" s="5"/>
       <c r="I147" s="5"/>
-    </row>
-    <row r="148" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J147" s="5"/>
+    </row>
+    <row r="148" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="2"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
@@ -2842,8 +3004,9 @@
       <c r="G148" s="2"/>
       <c r="H148" s="2"/>
       <c r="I148" s="2"/>
-    </row>
-    <row r="149" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J148" s="2"/>
+    </row>
+    <row r="149" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="5"/>
       <c r="B149" s="5"/>
       <c r="C149" s="5"/>
@@ -2853,8 +3016,9 @@
       <c r="G149" s="5"/>
       <c r="H149" s="5"/>
       <c r="I149" s="5"/>
-    </row>
-    <row r="150" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J149" s="5"/>
+    </row>
+    <row r="150" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="2"/>
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
@@ -2864,8 +3028,9 @@
       <c r="G150" s="2"/>
       <c r="H150" s="2"/>
       <c r="I150" s="2"/>
-    </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J150" s="2"/>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A151" s="5"/>
       <c r="B151" s="5"/>
       <c r="C151" s="5"/>
@@ -2875,8 +3040,9 @@
       <c r="G151" s="5"/>
       <c r="H151" s="5"/>
       <c r="I151" s="5"/>
-    </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J151" s="5"/>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A152" s="5"/>
       <c r="B152" s="5"/>
       <c r="C152" s="5"/>
@@ -2886,8 +3052,9 @@
       <c r="G152" s="5"/>
       <c r="H152" s="5"/>
       <c r="I152" s="5"/>
-    </row>
-    <row r="153" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J152" s="5"/>
+    </row>
+    <row r="153" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="2"/>
       <c r="B153" s="2"/>
       <c r="C153" s="2"/>
@@ -2897,8 +3064,9 @@
       <c r="G153" s="2"/>
       <c r="H153" s="2"/>
       <c r="I153" s="2"/>
-    </row>
-    <row r="154" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J153" s="2"/>
+    </row>
+    <row r="154" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="2"/>
       <c r="B154" s="2"/>
       <c r="C154" s="2"/>
@@ -2908,8 +3076,9 @@
       <c r="G154" s="2"/>
       <c r="H154" s="2"/>
       <c r="I154" s="2"/>
-    </row>
-    <row r="155" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J154" s="2"/>
+    </row>
+    <row r="155" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="2"/>
       <c r="B155" s="2"/>
       <c r="C155" s="2"/>
@@ -2919,8 +3088,9 @@
       <c r="G155" s="2"/>
       <c r="H155" s="2"/>
       <c r="I155" s="2"/>
-    </row>
-    <row r="156" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J155" s="2"/>
+    </row>
+    <row r="156" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="5"/>
       <c r="B156" s="5"/>
       <c r="C156" s="5"/>
@@ -2930,8 +3100,9 @@
       <c r="G156" s="5"/>
       <c r="H156" s="5"/>
       <c r="I156" s="5"/>
-    </row>
-    <row r="157" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J156" s="5"/>
+    </row>
+    <row r="157" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="2"/>
       <c r="B157" s="2"/>
       <c r="C157" s="2"/>
@@ -2941,8 +3112,9 @@
       <c r="G157" s="2"/>
       <c r="H157" s="2"/>
       <c r="I157" s="2"/>
-    </row>
-    <row r="158" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J157" s="2"/>
+    </row>
+    <row r="158" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="2"/>
       <c r="B158" s="2"/>
       <c r="C158" s="2"/>
@@ -2952,8 +3124,9 @@
       <c r="G158" s="2"/>
       <c r="H158" s="2"/>
       <c r="I158" s="2"/>
-    </row>
-    <row r="159" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J158" s="2"/>
+    </row>
+    <row r="159" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="2"/>
       <c r="B159" s="2"/>
       <c r="C159" s="2"/>
@@ -2963,8 +3136,9 @@
       <c r="G159" s="2"/>
       <c r="H159" s="2"/>
       <c r="I159" s="2"/>
-    </row>
-    <row r="160" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J159" s="2"/>
+    </row>
+    <row r="160" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="2"/>
       <c r="B160" s="2"/>
       <c r="C160" s="2"/>
@@ -2974,8 +3148,9 @@
       <c r="G160" s="2"/>
       <c r="H160" s="2"/>
       <c r="I160" s="2"/>
-    </row>
-    <row r="161" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J160" s="2"/>
+    </row>
+    <row r="161" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="2"/>
       <c r="B161" s="2"/>
       <c r="C161" s="2"/>
@@ -2985,8 +3160,9 @@
       <c r="G161" s="2"/>
       <c r="H161" s="2"/>
       <c r="I161" s="2"/>
-    </row>
-    <row r="162" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J161" s="2"/>
+    </row>
+    <row r="162" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="2"/>
       <c r="B162" s="2"/>
       <c r="C162" s="2"/>
@@ -2994,9 +3170,10 @@
       <c r="E162" s="2"/>
       <c r="F162" s="2"/>
       <c r="G162" s="2"/>
-      <c r="I162" s="2"/>
-    </row>
-    <row r="163" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H162" s="2"/>
+      <c r="J162" s="2"/>
+    </row>
+    <row r="163" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="2"/>
       <c r="B163" s="2"/>
       <c r="C163" s="2"/>
@@ -3006,8 +3183,9 @@
       <c r="G163" s="2"/>
       <c r="H163" s="2"/>
       <c r="I163" s="2"/>
-    </row>
-    <row r="164" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J163" s="2"/>
+    </row>
+    <row r="164" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="2"/>
       <c r="B164" s="2"/>
       <c r="C164" s="2"/>
@@ -3017,8 +3195,9 @@
       <c r="G164" s="2"/>
       <c r="H164" s="2"/>
       <c r="I164" s="2"/>
-    </row>
-    <row r="165" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J164" s="2"/>
+    </row>
+    <row r="165" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="2"/>
       <c r="B165" s="2"/>
       <c r="C165" s="2"/>
@@ -3028,8 +3207,9 @@
       <c r="G165" s="2"/>
       <c r="H165" s="2"/>
       <c r="I165" s="2"/>
-    </row>
-    <row r="166" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J165" s="2"/>
+    </row>
+    <row r="166" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="2"/>
       <c r="B166" s="2"/>
       <c r="C166" s="2"/>
@@ -3039,8 +3219,9 @@
       <c r="G166" s="2"/>
       <c r="H166" s="2"/>
       <c r="I166" s="2"/>
-    </row>
-    <row r="167" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J166" s="2"/>
+    </row>
+    <row r="167" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="2"/>
       <c r="B167" s="2"/>
       <c r="C167" s="2"/>
@@ -3050,8 +3231,9 @@
       <c r="G167" s="2"/>
       <c r="H167" s="2"/>
       <c r="I167" s="2"/>
-    </row>
-    <row r="168" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J167" s="2"/>
+    </row>
+    <row r="168" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="2"/>
       <c r="B168" s="2"/>
       <c r="C168" s="2"/>
@@ -3061,8 +3243,9 @@
       <c r="G168" s="2"/>
       <c r="H168" s="2"/>
       <c r="I168" s="2"/>
-    </row>
-    <row r="169" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J168" s="2"/>
+    </row>
+    <row r="169" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="2"/>
       <c r="B169" s="2"/>
       <c r="C169" s="2"/>
@@ -3072,8 +3255,9 @@
       <c r="G169" s="2"/>
       <c r="H169" s="2"/>
       <c r="I169" s="2"/>
-    </row>
-    <row r="170" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J169" s="2"/>
+    </row>
+    <row r="170" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="2"/>
       <c r="B170" s="2"/>
       <c r="C170" s="2"/>
@@ -3083,8 +3267,9 @@
       <c r="G170" s="2"/>
       <c r="H170" s="2"/>
       <c r="I170" s="2"/>
-    </row>
-    <row r="171" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J170" s="2"/>
+    </row>
+    <row r="171" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="2"/>
       <c r="B171" s="2"/>
       <c r="C171" s="2"/>
@@ -3094,8 +3279,9 @@
       <c r="G171" s="2"/>
       <c r="H171" s="2"/>
       <c r="I171" s="2"/>
-    </row>
-    <row r="172" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J171" s="2"/>
+    </row>
+    <row r="172" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="2"/>
       <c r="B172" s="2"/>
       <c r="C172" s="2"/>
@@ -3105,8 +3291,9 @@
       <c r="G172" s="2"/>
       <c r="H172" s="2"/>
       <c r="I172" s="2"/>
-    </row>
-    <row r="173" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J172" s="2"/>
+    </row>
+    <row r="173" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="2"/>
       <c r="B173" s="2"/>
       <c r="C173" s="2"/>
@@ -3116,8 +3303,9 @@
       <c r="G173" s="2"/>
       <c r="H173" s="2"/>
       <c r="I173" s="2"/>
-    </row>
-    <row r="174" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J173" s="2"/>
+    </row>
+    <row r="174" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="2"/>
       <c r="B174" s="2"/>
       <c r="C174" s="2"/>
@@ -3127,8 +3315,9 @@
       <c r="G174" s="2"/>
       <c r="H174" s="2"/>
       <c r="I174" s="2"/>
-    </row>
-    <row r="175" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J174" s="2"/>
+    </row>
+    <row r="175" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="2"/>
       <c r="B175" s="2"/>
       <c r="C175" s="2"/>
@@ -3138,8 +3327,9 @@
       <c r="G175" s="2"/>
       <c r="H175" s="2"/>
       <c r="I175" s="2"/>
-    </row>
-    <row r="176" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J175" s="2"/>
+    </row>
+    <row r="176" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="2"/>
       <c r="B176" s="2"/>
       <c r="C176" s="2"/>
@@ -3149,8 +3339,9 @@
       <c r="G176" s="2"/>
       <c r="H176" s="2"/>
       <c r="I176" s="2"/>
-    </row>
-    <row r="177" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J176" s="2"/>
+    </row>
+    <row r="177" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="2"/>
       <c r="B177" s="2"/>
       <c r="C177" s="2"/>
@@ -3160,8 +3351,9 @@
       <c r="G177" s="2"/>
       <c r="H177" s="2"/>
       <c r="I177" s="2"/>
-    </row>
-    <row r="178" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J177" s="2"/>
+    </row>
+    <row r="178" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="2"/>
       <c r="B178" s="2"/>
       <c r="C178" s="2"/>
@@ -3171,8 +3363,9 @@
       <c r="G178" s="2"/>
       <c r="H178" s="2"/>
       <c r="I178" s="2"/>
-    </row>
-    <row r="179" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J178" s="2"/>
+    </row>
+    <row r="179" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="2"/>
       <c r="B179" s="2"/>
       <c r="C179" s="2"/>
@@ -3182,8 +3375,9 @@
       <c r="G179" s="2"/>
       <c r="H179" s="2"/>
       <c r="I179" s="2"/>
-    </row>
-    <row r="180" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J179" s="2"/>
+    </row>
+    <row r="180" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="2"/>
       <c r="B180" s="2"/>
       <c r="C180" s="2"/>
@@ -3193,8 +3387,9 @@
       <c r="G180" s="2"/>
       <c r="H180" s="2"/>
       <c r="I180" s="2"/>
-    </row>
-    <row r="181" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J180" s="2"/>
+    </row>
+    <row r="181" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="2"/>
       <c r="B181" s="2"/>
       <c r="C181" s="2"/>
@@ -3204,8 +3399,9 @@
       <c r="G181" s="2"/>
       <c r="H181" s="2"/>
       <c r="I181" s="2"/>
-    </row>
-    <row r="182" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J181" s="2"/>
+    </row>
+    <row r="182" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="2"/>
       <c r="B182" s="2"/>
       <c r="C182" s="2"/>
@@ -3215,8 +3411,9 @@
       <c r="G182" s="2"/>
       <c r="H182" s="2"/>
       <c r="I182" s="2"/>
-    </row>
-    <row r="183" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J182" s="2"/>
+    </row>
+    <row r="183" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="2"/>
       <c r="B183" s="2"/>
       <c r="C183" s="2"/>
@@ -3226,8 +3423,9 @@
       <c r="G183" s="2"/>
       <c r="H183" s="2"/>
       <c r="I183" s="2"/>
-    </row>
-    <row r="184" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J183" s="2"/>
+    </row>
+    <row r="184" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="2"/>
       <c r="B184" s="2"/>
       <c r="C184" s="2"/>
@@ -3237,8 +3435,9 @@
       <c r="G184" s="2"/>
       <c r="H184" s="2"/>
       <c r="I184" s="2"/>
-    </row>
-    <row r="185" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J184" s="2"/>
+    </row>
+    <row r="185" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" s="6"/>
       <c r="B185" s="6"/>
       <c r="C185" s="6"/>
@@ -3265,8 +3464,9 @@
       <c r="X185" s="6"/>
       <c r="Y185" s="6"/>
       <c r="Z185" s="6"/>
-    </row>
-    <row r="186" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA185" s="6"/>
+    </row>
+    <row r="186" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" s="2"/>
       <c r="B186" s="2"/>
       <c r="C186" s="2"/>
@@ -3293,8 +3493,9 @@
       <c r="X186" s="2"/>
       <c r="Y186" s="2"/>
       <c r="Z186" s="2"/>
-    </row>
-    <row r="187" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA186" s="2"/>
+    </row>
+    <row r="187" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" s="2"/>
       <c r="B187" s="2"/>
       <c r="C187" s="2"/>
@@ -3304,8 +3505,9 @@
       <c r="G187" s="2"/>
       <c r="H187" s="2"/>
       <c r="I187" s="2"/>
-    </row>
-    <row r="188" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J187" s="2"/>
+    </row>
+    <row r="188" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="2"/>
       <c r="B188" s="2"/>
       <c r="C188" s="2"/>
@@ -3315,8 +3517,9 @@
       <c r="G188" s="2"/>
       <c r="H188" s="2"/>
       <c r="I188" s="2"/>
-    </row>
-    <row r="189" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J188" s="2"/>
+    </row>
+    <row r="189" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="5"/>
       <c r="B189" s="5"/>
       <c r="C189" s="5"/>
@@ -3326,8 +3529,9 @@
       <c r="G189" s="5"/>
       <c r="H189" s="5"/>
       <c r="I189" s="5"/>
-    </row>
-    <row r="190" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J189" s="5"/>
+    </row>
+    <row r="190" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" s="5"/>
       <c r="B190" s="5"/>
       <c r="C190" s="5"/>
@@ -3337,12 +3541,13 @@
       <c r="G190" s="5"/>
       <c r="H190" s="5"/>
       <c r="I190" s="5"/>
-    </row>
-    <row r="191" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J190" s="5"/>
+    </row>
+    <row r="191" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" s="6"/>
       <c r="B191" s="6"/>
       <c r="C191" s="5"/>
-      <c r="D191" s="6"/>
+      <c r="D191" s="5"/>
       <c r="E191" s="6"/>
       <c r="F191" s="6"/>
       <c r="G191" s="6"/>
@@ -3365,8 +3570,9 @@
       <c r="X191" s="6"/>
       <c r="Y191" s="6"/>
       <c r="Z191" s="6"/>
-    </row>
-    <row r="192" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA191" s="6"/>
+    </row>
+    <row r="192" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="5"/>
       <c r="B192" s="5"/>
       <c r="C192" s="5"/>
@@ -3376,8 +3582,9 @@
       <c r="G192" s="5"/>
       <c r="H192" s="5"/>
       <c r="I192" s="5"/>
-    </row>
-    <row r="193" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J192" s="5"/>
+    </row>
+    <row r="193" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="5"/>
       <c r="B193" s="5"/>
       <c r="C193" s="5"/>
@@ -3387,8 +3594,9 @@
       <c r="G193" s="5"/>
       <c r="H193" s="5"/>
       <c r="I193" s="5"/>
-    </row>
-    <row r="194" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J193" s="5"/>
+    </row>
+    <row r="194" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="5"/>
       <c r="B194" s="5"/>
       <c r="C194" s="5"/>
@@ -3398,8 +3606,9 @@
       <c r="G194" s="5"/>
       <c r="H194" s="5"/>
       <c r="I194" s="5"/>
-    </row>
-    <row r="195" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J194" s="5"/>
+    </row>
+    <row r="195" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" s="5"/>
       <c r="B195" s="5"/>
       <c r="C195" s="5"/>
@@ -3409,8 +3618,9 @@
       <c r="G195" s="5"/>
       <c r="H195" s="5"/>
       <c r="I195" s="5"/>
-    </row>
-    <row r="196" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J195" s="5"/>
+    </row>
+    <row r="196" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" s="5"/>
       <c r="B196" s="5"/>
       <c r="C196" s="5"/>
@@ -3420,8 +3630,9 @@
       <c r="G196" s="5"/>
       <c r="H196" s="5"/>
       <c r="I196" s="5"/>
-    </row>
-    <row r="197" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J196" s="5"/>
+    </row>
+    <row r="197" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" s="5"/>
       <c r="B197" s="5"/>
       <c r="C197" s="5"/>
@@ -3431,7 +3642,7 @@
       <c r="G197" s="5"/>
       <c r="H197" s="5"/>
       <c r="I197" s="5"/>
-      <c r="J197" s="2"/>
+      <c r="J197" s="5"/>
       <c r="K197" s="2"/>
       <c r="L197" s="2"/>
       <c r="M197" s="2"/>
@@ -3448,8 +3659,9 @@
       <c r="X197" s="2"/>
       <c r="Y197" s="2"/>
       <c r="Z197" s="2"/>
-    </row>
-    <row r="198" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA197" s="2"/>
+    </row>
+    <row r="198" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="5"/>
       <c r="B198" s="5"/>
       <c r="C198" s="5"/>
@@ -3459,8 +3671,9 @@
       <c r="G198" s="5"/>
       <c r="H198" s="5"/>
       <c r="I198" s="5"/>
-    </row>
-    <row r="199" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J198" s="5"/>
+    </row>
+    <row r="199" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="5"/>
       <c r="B199" s="5"/>
       <c r="C199" s="5"/>
@@ -3470,8 +3683,9 @@
       <c r="G199" s="5"/>
       <c r="H199" s="5"/>
       <c r="I199" s="5"/>
-    </row>
-    <row r="200" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J199" s="5"/>
+    </row>
+    <row r="200" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="5"/>
       <c r="B200" s="5"/>
       <c r="C200" s="5"/>
@@ -3481,8 +3695,9 @@
       <c r="G200" s="5"/>
       <c r="H200" s="5"/>
       <c r="I200" s="5"/>
-    </row>
-    <row r="201" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J200" s="5"/>
+    </row>
+    <row r="201" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" s="5"/>
       <c r="B201" s="5"/>
       <c r="C201" s="5"/>
@@ -3492,8 +3707,9 @@
       <c r="G201" s="5"/>
       <c r="H201" s="5"/>
       <c r="I201" s="5"/>
-    </row>
-    <row r="202" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J201" s="5"/>
+    </row>
+    <row r="202" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" s="5"/>
       <c r="B202" s="5"/>
       <c r="C202" s="5"/>
@@ -3503,8 +3719,9 @@
       <c r="G202" s="5"/>
       <c r="H202" s="5"/>
       <c r="I202" s="5"/>
-    </row>
-    <row r="203" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J202" s="5"/>
+    </row>
+    <row r="203" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="5"/>
       <c r="B203" s="5"/>
       <c r="C203" s="5"/>
@@ -3514,8 +3731,9 @@
       <c r="G203" s="5"/>
       <c r="H203" s="5"/>
       <c r="I203" s="5"/>
-    </row>
-    <row r="204" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J203" s="5"/>
+    </row>
+    <row r="204" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="5"/>
       <c r="B204" s="5"/>
       <c r="C204" s="5"/>
@@ -3525,8 +3743,9 @@
       <c r="G204" s="5"/>
       <c r="H204" s="5"/>
       <c r="I204" s="5"/>
-    </row>
-    <row r="205" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J204" s="5"/>
+    </row>
+    <row r="205" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="5"/>
       <c r="B205" s="5"/>
       <c r="C205" s="5"/>
@@ -3536,8 +3755,9 @@
       <c r="G205" s="5"/>
       <c r="H205" s="5"/>
       <c r="I205" s="5"/>
-    </row>
-    <row r="206" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J205" s="5"/>
+    </row>
+    <row r="206" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" s="5"/>
       <c r="B206" s="5"/>
       <c r="C206" s="5"/>
@@ -3547,8 +3767,9 @@
       <c r="G206" s="5"/>
       <c r="H206" s="5"/>
       <c r="I206" s="5"/>
-    </row>
-    <row r="207" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J206" s="5"/>
+    </row>
+    <row r="207" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" s="2"/>
       <c r="B207" s="2"/>
       <c r="C207" s="2"/>
@@ -3558,8 +3779,9 @@
       <c r="G207" s="2"/>
       <c r="H207" s="2"/>
       <c r="I207" s="2"/>
-    </row>
-    <row r="208" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J207" s="2"/>
+    </row>
+    <row r="208" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" s="2"/>
       <c r="B208" s="2"/>
       <c r="C208" s="2"/>
@@ -3569,8 +3791,9 @@
       <c r="G208" s="2"/>
       <c r="H208" s="2"/>
       <c r="I208" s="2"/>
-    </row>
-    <row r="209" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J208" s="2"/>
+    </row>
+    <row r="209" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="2"/>
       <c r="B209" s="2"/>
       <c r="C209" s="2"/>
@@ -3580,8 +3803,9 @@
       <c r="G209" s="2"/>
       <c r="H209" s="2"/>
       <c r="I209" s="2"/>
-    </row>
-    <row r="210" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J209" s="2"/>
+    </row>
+    <row r="210" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" s="2"/>
       <c r="B210" s="2"/>
       <c r="C210" s="2"/>
@@ -3591,8 +3815,9 @@
       <c r="G210" s="2"/>
       <c r="H210" s="2"/>
       <c r="I210" s="2"/>
-    </row>
-    <row r="211" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J210" s="2"/>
+    </row>
+    <row r="211" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" s="2"/>
       <c r="B211" s="2"/>
       <c r="C211" s="2"/>
@@ -3602,8 +3827,9 @@
       <c r="G211" s="2"/>
       <c r="H211" s="2"/>
       <c r="I211" s="2"/>
-    </row>
-    <row r="212" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J211" s="2"/>
+    </row>
+    <row r="212" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" s="2"/>
       <c r="B212" s="2"/>
       <c r="C212" s="2"/>
@@ -3613,8 +3839,9 @@
       <c r="G212" s="2"/>
       <c r="H212" s="2"/>
       <c r="I212" s="2"/>
-    </row>
-    <row r="213" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J212" s="2"/>
+    </row>
+    <row r="213" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" s="2"/>
       <c r="B213" s="2"/>
       <c r="C213" s="2"/>
@@ -3624,8 +3851,9 @@
       <c r="G213" s="2"/>
       <c r="H213" s="2"/>
       <c r="I213" s="2"/>
-    </row>
-    <row r="214" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J213" s="2"/>
+    </row>
+    <row r="214" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A214" s="2"/>
       <c r="B214" s="2"/>
       <c r="C214" s="2"/>
@@ -3635,8 +3863,9 @@
       <c r="G214" s="2"/>
       <c r="H214" s="2"/>
       <c r="I214" s="2"/>
-    </row>
-    <row r="215" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J214" s="2"/>
+    </row>
+    <row r="215" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A215" s="2"/>
       <c r="B215" s="2"/>
       <c r="C215" s="2"/>
@@ -3646,8 +3875,9 @@
       <c r="G215" s="2"/>
       <c r="H215" s="2"/>
       <c r="I215" s="2"/>
-    </row>
-    <row r="216" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J215" s="2"/>
+    </row>
+    <row r="216" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A216" s="2"/>
       <c r="B216" s="2"/>
       <c r="C216" s="2"/>
@@ -3657,8 +3887,9 @@
       <c r="G216" s="2"/>
       <c r="H216" s="2"/>
       <c r="I216" s="2"/>
-    </row>
-    <row r="217" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J216" s="2"/>
+    </row>
+    <row r="217" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A217" s="5"/>
       <c r="B217" s="5"/>
       <c r="C217" s="5"/>
@@ -3668,8 +3899,9 @@
       <c r="G217" s="5"/>
       <c r="H217" s="5"/>
       <c r="I217" s="5"/>
-    </row>
-    <row r="218" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J217" s="5"/>
+    </row>
+    <row r="218" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A218" s="5"/>
       <c r="B218" s="5"/>
       <c r="C218" s="5"/>
@@ -3679,8 +3911,9 @@
       <c r="G218" s="5"/>
       <c r="H218" s="5"/>
       <c r="I218" s="5"/>
-    </row>
-    <row r="219" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J218" s="5"/>
+    </row>
+    <row r="219" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A219" s="5"/>
       <c r="B219" s="5"/>
       <c r="C219" s="5"/>
@@ -3690,8 +3923,9 @@
       <c r="G219" s="5"/>
       <c r="H219" s="5"/>
       <c r="I219" s="5"/>
-    </row>
-    <row r="220" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J219" s="5"/>
+    </row>
+    <row r="220" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A220" s="5"/>
       <c r="B220" s="5"/>
       <c r="C220" s="5"/>
@@ -3701,8 +3935,9 @@
       <c r="G220" s="5"/>
       <c r="H220" s="5"/>
       <c r="I220" s="5"/>
-    </row>
-    <row r="221" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J220" s="5"/>
+    </row>
+    <row r="221" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" s="5"/>
       <c r="B221" s="5"/>
       <c r="C221" s="5"/>
@@ -3712,201 +3947,202 @@
       <c r="G221" s="5"/>
       <c r="H221" s="5"/>
       <c r="I221" s="5"/>
-    </row>
-    <row r="222" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="223" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="224" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="225" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="226" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="227" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="228" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="229" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="230" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="231" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="232" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="233" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="234" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="235" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="236" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="237" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="238" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="239" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="240" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="241" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="242" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="243" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="244" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="245" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="246" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="247" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="248" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="249" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="250" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="251" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="252" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="253" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="254" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="255" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="256" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="257" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="258" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="259" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="260" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="261" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="262" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="263" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="264" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="265" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="266" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="267" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="268" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="269" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="270" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="271" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="272" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="273" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="274" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="275" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="276" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="277" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="278" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="279" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="280" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="281" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="282" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="283" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="284" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="285" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="286" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="287" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="288" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="289" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="290" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="291" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="292" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="293" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="294" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="295" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="296" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="297" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="298" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="299" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="300" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="301" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="302" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="303" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="304" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="305" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="306" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="307" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="308" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="309" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="310" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="311" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="312" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="313" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="314" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="315" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="316" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="317" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="318" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="319" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="320" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="321" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="322" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="323" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="324" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="325" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="326" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="327" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="328" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="329" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="330" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="331" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="332" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="333" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="334" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="335" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="336" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="337" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="338" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="339" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="340" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="341" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="342" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="343" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="344" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="345" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="346" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="347" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="348" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="349" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="350" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="351" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="352" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="353" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="354" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="355" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="356" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="357" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="358" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="359" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="360" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="361" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="362" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="363" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="364" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="365" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="366" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="367" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="368" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="369" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="370" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="371" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="372" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="373" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="374" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="375" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="376" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="377" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="378" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="379" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="380" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="381" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="382" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="383" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="384" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="385" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="386" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="387" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="388" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="389" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="390" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="391" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="392" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="393" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="394" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="395" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="396" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="397" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="398" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="399" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="400" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="401" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="402" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="403" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="404" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="405" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="406" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="407" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="408" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="409" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="410" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="411" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="412" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="413" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="414" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="415" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="J221" s="5"/>
+    </row>
+    <row r="222" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="223" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="224" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="225" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="226" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="227" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="228" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="229" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="230" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="231" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="232" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="233" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="234" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="235" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="236" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="237" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="238" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="239" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="240" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="241" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="242" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="243" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="244" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="245" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="246" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="247" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="248" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="249" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="250" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="251" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="252" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="253" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="254" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="255" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="256" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="257" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="258" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="259" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="260" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="261" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="262" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="263" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="264" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="265" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="266" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="267" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="268" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="269" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="270" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="271" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="272" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="273" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="274" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="275" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="276" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="277" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="278" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="279" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="280" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="281" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="282" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="283" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="284" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="285" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="286" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="287" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="288" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="289" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="290" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="291" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="292" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="293" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="294" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="295" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="296" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="297" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="298" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="299" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="300" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="301" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="302" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="303" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="304" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="305" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="306" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="307" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="308" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="309" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="310" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="311" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="312" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="313" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="314" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="315" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="316" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="317" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="318" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="319" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="320" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="321" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="322" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="323" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="324" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="325" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="326" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="327" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="328" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="329" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="330" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="331" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="332" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="333" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="334" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="335" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="336" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="337" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="338" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="339" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="340" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="341" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="342" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="343" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="344" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="345" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="346" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="347" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="348" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="349" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="350" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="351" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="352" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="353" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="354" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="355" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="356" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="357" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="358" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="359" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="360" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="361" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="362" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="363" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="364" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="365" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="366" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="367" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="368" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="369" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="370" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="371" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="372" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="373" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="374" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="375" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="376" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="377" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="378" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="379" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="380" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="381" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="382" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="383" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="384" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="385" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="386" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="387" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="388" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="389" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="390" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="391" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="392" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="393" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="394" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="395" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="396" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="397" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="398" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="399" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="400" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="401" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="402" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="403" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="404" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="405" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="406" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="407" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="408" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="409" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="410" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="411" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="412" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="413" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="414" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="415" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="416" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="417" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="418" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4559,11 +4795,11 @@
     <row r="1065" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1066" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <autoFilter ref="A1:Z221" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AA221" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{543D5F22-D32D-2F40-9C06-08DB464A3DC9}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{A3E2A82B-9C7B-E346-B1CE-3B49FB9DF51F}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{C1F5CB4D-9CB0-B847-A249-98565601C11A}"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{543D5F22-D32D-2F40-9C06-08DB464A3DC9}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{A3E2A82B-9C7B-E346-B1CE-3B49FB9DF51F}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{C1F5CB4D-9CB0-B847-A249-98565601C11A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -18347,4 +18583,10 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{e9c55f1f-f169-4db7-a264-a5084ccbb748}" enabled="1" method="Standard" siteId="{135e8995-7d3b-4466-844b-a0d62ba5f495}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>